<commit_message>
Updated the project successfully
</commit_message>
<xml_diff>
--- a/com.billingProject/src/test/resources/ExcellBilling.xlsx
+++ b/com.billingProject/src/test/resources/ExcellBilling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shabi\eclipse-workspace\com.bilingProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shabi\git\Project-Automation\com.billingProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA81391-7E76-46A9-831A-015F8D045E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4B54D5-B3DC-4F8F-A980-A04933FD96EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11736" yWindow="3360" windowWidth="11304" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>No matching records</t>
   </si>
   <si>
-    <t>Meenakshi</t>
-  </si>
-  <si>
     <t>verifyColumnVisibilityFunctionality</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>Sushil</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,7 +658,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3"/>
     </row>
@@ -667,13 +667,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>